<commit_message>
pipe info for control
</commit_message>
<xml_diff>
--- a/doc/dependencies_pipeline.xlsx
+++ b/doc/dependencies_pipeline.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="660" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="7050" yWindow="660" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="idea pipeline" sheetId="3" r:id="rId1"/>
     <sheet name="RAW" sheetId="1" r:id="rId2"/>
     <sheet name="pipeline behaviour" sheetId="2" r:id="rId3"/>
+    <sheet name="idea pipeline 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="46">
   <si>
     <t>lw v1, 0(v1)</t>
   </si>
@@ -103,13 +104,64 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Data Processing</t>
+  </si>
+  <si>
+    <t>EX1</t>
+  </si>
+  <si>
+    <t>EX2</t>
+  </si>
+  <si>
+    <t>EX3</t>
+  </si>
+  <si>
+    <t>EX4</t>
+  </si>
+  <si>
+    <t>Data Transfer</t>
+  </si>
+  <si>
+    <t>Write Data Memory</t>
+  </si>
+  <si>
+    <t>ADR</t>
+  </si>
+  <si>
+    <t>DM1</t>
+  </si>
+  <si>
+    <t>DM2</t>
+  </si>
+  <si>
+    <t>Read Data Memory</t>
+  </si>
+  <si>
+    <t>Program Control</t>
+  </si>
+  <si>
+    <t>Compare</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Compare Branch</t>
+  </si>
+  <si>
+    <t>* Make pipeline stages of read write data uniform with read write data offset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +175,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +223,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -268,6 +351,35 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1243,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A3:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1257,11 +1369,6 @@
     <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>13</v>
@@ -1380,4 +1487,266 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="20" width="5.7109375" style="21" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="20">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20">
+        <v>6</v>
+      </c>
+      <c r="H1" s="20">
+        <v>7</v>
+      </c>
+      <c r="I1" s="20">
+        <v>8</v>
+      </c>
+      <c r="J1" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="19"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>